<commit_message>
Add process update description
- elaborate Annex 4 example
- changed versioning of route sections in all examples
- regenerate all graphs and excel sheets
</commit_message>
<xml_diff>
--- a/docs/examples/train-TR-12AB-1.xlsx
+++ b/docs/examples/train-TR-12AB-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\tap-tsi\fte-tom\tom\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\tap-tsi\fte-tom\tom\docs\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4291DC99-22E9-4D06-B9F1-61CC7273EC51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9B42764-9205-4AA0-A657-86C2A46CE2BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6630" yWindow="840" windowWidth="29040" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,97 +34,97 @@
     <t>FF</t>
   </si>
   <si>
-    <t>TR/8350/12AB/00/1/2021-12-01</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-02</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-03</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-04</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-05</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-06</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-07</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-08</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-09</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-10</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-11</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-12</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-13</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-14</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-15</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-16</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-17</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-18</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-19</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-20</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-21</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-22</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-23</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-24</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-25</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-26</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-27</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-28</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-29</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/1/2021-12-30</t>
-  </si>
-  <si>
-    <t>TR/8350/12AB/00/3/2021-12-31</t>
+    <t>TR/8350/12AB/2021/10.01/2021-12-01</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-02</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-03</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-04</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-05</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-06</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-07</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-08</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-09</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-10</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-11</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-12</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-13</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-14</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-15</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-16</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-17</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-18</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-19</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-20</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-21</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-22</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-23</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-24</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-25</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-26</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-27</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-28</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-29</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/10.01/2021-12-30</t>
+  </si>
+  <si>
+    <t>TR/8350/12AB/2021/20.01/2021-12-31</t>
   </si>
 </sst>
 </file>
@@ -132,7 +132,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -146,7 +146,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -189,7 +188,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -494,14 +493,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>